<commit_message>
Changed a lot of the game board, got lines somewhat working, need to fix up game board more.
</commit_message>
<xml_diff>
--- a/Board Measurements.xlsx
+++ b/Board Measurements.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B68F8-DF40-4A09-8AA2-B98F0E5FB392}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB23E75-EFD0-42F8-92FF-06E5958C8F12}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,7 +210,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -243,10 +243,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52:I52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,10 +541,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="2"/>
       <c r="D4" t="s">
         <v>1</v>
       </c>
@@ -569,7 +569,7 @@
         <v>55</v>
       </c>
       <c r="B5">
-        <v>850</v>
+        <v>800</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
@@ -578,18 +578,18 @@
         <v>3</v>
       </c>
       <c r="F5">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="G5">
-        <v>208</v>
-      </c>
-      <c r="H5" s="2">
+        <v>107</v>
+      </c>
+      <c r="H5" s="1">
         <f>F5/$B$5</f>
-        <v>8.352941176470588E-2</v>
-      </c>
-      <c r="I5" s="2">
-        <f>G5/$B$5</f>
-        <v>0.24470588235294119</v>
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <f>G5/$B$6</f>
+        <v>0.26097560975609757</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>56</v>
       </c>
       <c r="B6">
-        <v>601</v>
+        <v>410</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -606,18 +606,18 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="G6">
-        <v>187</v>
-      </c>
-      <c r="H6" s="2">
+        <v>85</v>
+      </c>
+      <c r="H6" s="1">
         <f t="shared" ref="H6:H52" si="0">F6/$B$5</f>
-        <v>0.17176470588235293</v>
-      </c>
-      <c r="I6" s="2">
-        <f t="shared" ref="I6:I52" si="1">G6/$B$5</f>
-        <v>0.22</v>
+        <v>0.15</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I52" si="1">G6/$B$6</f>
+        <v>0.2073170731707317</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -628,18 +628,18 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="G7">
-        <v>230</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
-        <v>0.1976470588235294</v>
-      </c>
-      <c r="I7" s="2">
-        <f t="shared" si="1"/>
-        <v>0.27058823529411763</v>
+        <v>128</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.17874999999999999</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31219512195121951</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -650,18 +650,18 @@
         <v>3</v>
       </c>
       <c r="F8">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="G8">
-        <v>185</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-      <c r="I8" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21764705882352942</v>
+        <v>83</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.20243902439024392</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -672,18 +672,18 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="G9">
-        <v>228</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.27058823529411763</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26823529411764707</v>
+        <v>125</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25624999999999998</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.3048780487804878</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -694,18 +694,18 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="G10">
-        <v>192</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="0"/>
-        <v>0.29411764705882354</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22588235294117648</v>
+        <v>89</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.21707317073170732</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -716,18 +716,18 @@
         <v>3</v>
       </c>
       <c r="F11">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="G11">
-        <v>156</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>0.42117647058823532</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="1"/>
-        <v>0.18352941176470589</v>
+        <v>54</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41625000000000001</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13170731707317074</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -738,18 +738,18 @@
         <v>3</v>
       </c>
       <c r="F12">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="G12">
-        <v>214</v>
-      </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>0.41176470588235292</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>0.25176470588235295</v>
+        <v>112</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.40625</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.27317073170731709</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -760,18 +760,18 @@
         <v>3</v>
       </c>
       <c r="F13">
-        <v>402</v>
+        <v>377</v>
       </c>
       <c r="G13">
-        <v>186</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>0.47294117647058825</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21882352941176469</v>
+        <v>83</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.47125</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.20243902439024392</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -782,18 +782,18 @@
         <v>3</v>
       </c>
       <c r="F14">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="G14">
-        <v>148</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>0.48941176470588238</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>0.17411764705882352</v>
+        <v>44</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10731707317073171</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -804,18 +804,18 @@
         <v>3</v>
       </c>
       <c r="F15">
-        <v>441</v>
+        <v>416</v>
       </c>
       <c r="G15">
-        <v>174</v>
-      </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>0.51882352941176468</v>
-      </c>
-      <c r="I15" s="2">
-        <f t="shared" si="1"/>
-        <v>0.20470588235294118</v>
+        <v>72</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17560975609756097</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -826,18 +826,18 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>481</v>
+        <v>456</v>
       </c>
       <c r="G16">
-        <v>134</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.5658823529411765</v>
-      </c>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
-        <v>0.15764705882352942</v>
+        <v>32</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>7.8048780487804878E-2</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
@@ -848,18 +848,18 @@
         <v>27</v>
       </c>
       <c r="F17">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G17">
-        <v>267</v>
-      </c>
-      <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>9.7647058823529406E-2</v>
-      </c>
-      <c r="I17" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31411764705882356</v>
+        <v>165</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40243902439024393</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
@@ -870,18 +870,18 @@
         <v>27</v>
       </c>
       <c r="F18">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="G18">
-        <v>287</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>0.16117647058823528</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.33764705882352941</v>
+        <v>185</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.14124999999999999</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45121951219512196</v>
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
@@ -892,18 +892,18 @@
         <v>27</v>
       </c>
       <c r="F19">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="G19">
-        <v>278</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
-        <v>0.24</v>
-      </c>
-      <c r="I19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.32705882352941179</v>
+        <v>176</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22375</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.42926829268292682</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
@@ -914,18 +914,18 @@
         <v>27</v>
       </c>
       <c r="F20">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="G20">
-        <v>337</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.23411764705882354</v>
-      </c>
-      <c r="I20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.39647058823529413</v>
+        <v>235</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2175</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.57317073170731703</v>
       </c>
     </row>
     <row r="21" spans="4:9" x14ac:dyDescent="0.25">
@@ -936,18 +936,18 @@
         <v>27</v>
       </c>
       <c r="F21">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="G21">
-        <v>400</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>0.21058823529411766</v>
-      </c>
-      <c r="I21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.47058823529411764</v>
+        <v>298</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1925</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.72682926829268291</v>
       </c>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.25">
@@ -958,18 +958,18 @@
         <v>27</v>
       </c>
       <c r="F22">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="G22">
-        <v>465</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.22</v>
-      </c>
-      <c r="I22" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54705882352941182</v>
+        <v>363</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20374999999999999</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88536585365853659</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.25">
@@ -980,18 +980,18 @@
         <v>27</v>
       </c>
       <c r="F23">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="G23">
-        <v>454</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.29176470588235293</v>
-      </c>
-      <c r="I23" s="2">
-        <f t="shared" si="1"/>
-        <v>0.53411764705882347</v>
+        <v>352</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27875</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.85853658536585364</v>
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.25">
@@ -1002,18 +1002,18 @@
         <v>27</v>
       </c>
       <c r="F24">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="G24">
-        <v>410</v>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.33176470588235296</v>
-      </c>
-      <c r="I24" s="2">
-        <f t="shared" si="1"/>
-        <v>0.4823529411764706</v>
+        <v>307</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32124999999999998</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.74878048780487805</v>
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.25">
@@ -1024,18 +1024,18 @@
         <v>27</v>
       </c>
       <c r="F25">
-        <v>396</v>
+        <v>371</v>
       </c>
       <c r="G25">
-        <v>327</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.46588235294117647</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.38470588235294118</v>
+        <v>225</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46375</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.54878048780487809</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.25">
@@ -1046,18 +1046,18 @@
         <v>27</v>
       </c>
       <c r="F26">
-        <v>434</v>
+        <v>408</v>
       </c>
       <c r="G26">
-        <v>368</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="0"/>
-        <v>0.51058823529411768</v>
-      </c>
-      <c r="I26" s="2">
-        <f t="shared" si="1"/>
-        <v>0.43294117647058822</v>
+        <v>266</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.51</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.64878048780487807</v>
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.25">
@@ -1068,18 +1068,18 @@
         <v>27</v>
       </c>
       <c r="F27">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="G27">
-        <v>427</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54941176470588238</v>
-      </c>
-      <c r="I27" s="2">
-        <f t="shared" si="1"/>
-        <v>0.50235294117647056</v>
+        <v>325</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55125000000000002</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79268292682926833</v>
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.25">
@@ -1090,18 +1090,18 @@
         <v>27</v>
       </c>
       <c r="F28">
-        <v>471</v>
+        <v>446</v>
       </c>
       <c r="G28">
-        <v>316</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.55411764705882349</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="1"/>
-        <v>0.37176470588235294</v>
+        <v>214</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5575</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="1"/>
+        <v>0.52195121951219514</v>
       </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.25">
@@ -1112,18 +1112,18 @@
         <v>40</v>
       </c>
       <c r="F29">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="G29">
-        <v>247</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="0"/>
-        <v>0.48823529411764705</v>
-      </c>
-      <c r="I29" s="2">
-        <f t="shared" si="1"/>
-        <v>0.29058823529411765</v>
+        <v>145</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="1"/>
+        <v>0.35365853658536583</v>
       </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.25">
@@ -1134,18 +1134,18 @@
         <v>40</v>
       </c>
       <c r="F30">
-        <v>467</v>
+        <v>442</v>
       </c>
       <c r="G30">
-        <v>208</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54941176470588238</v>
-      </c>
-      <c r="I30" s="2">
-        <f t="shared" si="1"/>
-        <v>0.24470588235294119</v>
+        <v>107</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55249999999999999</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="1"/>
+        <v>0.26097560975609757</v>
       </c>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.25">
@@ -1156,18 +1156,18 @@
         <v>40</v>
       </c>
       <c r="F31">
-        <v>459</v>
+        <v>434</v>
       </c>
       <c r="G31">
-        <v>259</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="0"/>
-        <v>0.54</v>
-      </c>
-      <c r="I31" s="2">
-        <f t="shared" si="1"/>
-        <v>0.30470588235294116</v>
+        <v>157</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.54249999999999998</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38292682926829269</v>
       </c>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.25">
@@ -1178,18 +1178,18 @@
         <v>40</v>
       </c>
       <c r="F32">
-        <v>509</v>
+        <v>484</v>
       </c>
       <c r="G32">
-        <v>239</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" si="0"/>
-        <v>0.59882352941176475</v>
-      </c>
-      <c r="I32" s="2">
-        <f t="shared" si="1"/>
-        <v>0.28117647058823531</v>
+        <v>137</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="0"/>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33414634146341465</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.25">
@@ -1200,18 +1200,18 @@
         <v>40</v>
       </c>
       <c r="F33">
-        <v>513</v>
+        <v>488</v>
       </c>
       <c r="G33">
-        <v>174</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="0"/>
-        <v>0.60352941176470587</v>
-      </c>
-      <c r="I33" s="2">
-        <f t="shared" si="1"/>
-        <v>0.20470588235294118</v>
+        <v>72</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17560975609756097</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.25">
@@ -1222,18 +1222,18 @@
         <v>40</v>
       </c>
       <c r="F34">
-        <v>553</v>
+        <v>528</v>
       </c>
       <c r="G34">
-        <v>202</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="0"/>
-        <v>0.65058823529411769</v>
-      </c>
-      <c r="I34" s="2">
-        <f t="shared" si="1"/>
-        <v>0.23764705882352941</v>
+        <v>100</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24390243902439024</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.25">
@@ -1244,18 +1244,18 @@
         <v>40</v>
       </c>
       <c r="F35">
-        <v>516</v>
+        <v>491</v>
       </c>
       <c r="G35">
-        <v>292</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="0"/>
-        <v>0.60705882352941176</v>
-      </c>
-      <c r="I35" s="2">
-        <f t="shared" si="1"/>
-        <v>0.34352941176470586</v>
+        <v>190</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.61375000000000002</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="1"/>
+        <v>0.46341463414634149</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.25">
@@ -1266,18 +1266,18 @@
         <v>40</v>
       </c>
       <c r="F36">
-        <v>565</v>
+        <v>540</v>
       </c>
       <c r="G36">
-        <v>285</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="0"/>
-        <v>0.66470588235294115</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" si="1"/>
-        <v>0.3352941176470588</v>
+        <v>156</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38048780487804879</v>
       </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.25">
@@ -1288,18 +1288,18 @@
         <v>40</v>
       </c>
       <c r="F37">
-        <v>570</v>
+        <v>545</v>
       </c>
       <c r="G37">
-        <v>301</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" si="0"/>
-        <v>0.6705882352941176</v>
-      </c>
-      <c r="I37" s="2">
-        <f t="shared" si="1"/>
-        <v>0.35411764705882354</v>
+        <v>199</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="1"/>
+        <v>0.48536585365853657</v>
       </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.25">
@@ -1310,18 +1310,18 @@
         <v>40</v>
       </c>
       <c r="F38">
-        <v>608</v>
+        <v>583</v>
       </c>
       <c r="G38">
-        <v>241</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="0"/>
-        <v>0.71529411764705886</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" si="1"/>
-        <v>0.28352941176470586</v>
+        <v>139</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72875000000000001</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="1"/>
+        <v>0.33902439024390246</v>
       </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.25">
@@ -1332,18 +1332,18 @@
         <v>40</v>
       </c>
       <c r="F39">
-        <v>616</v>
+        <v>591</v>
       </c>
       <c r="G39">
-        <v>333</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="0"/>
-        <v>0.7247058823529412</v>
-      </c>
-      <c r="I39" s="2">
-        <f t="shared" si="1"/>
-        <v>0.39176470588235296</v>
+        <v>231</v>
+      </c>
+      <c r="H39" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73875000000000002</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="1"/>
+        <v>0.56341463414634141</v>
       </c>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.25">
@@ -1354,18 +1354,18 @@
         <v>40</v>
       </c>
       <c r="F40">
-        <v>649</v>
+        <v>624</v>
       </c>
       <c r="G40">
-        <v>255</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" si="0"/>
-        <v>0.7635294117647059</v>
-      </c>
-      <c r="I40" s="2">
-        <f t="shared" si="1"/>
-        <v>0.3</v>
+        <v>153</v>
+      </c>
+      <c r="H40" s="1">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37317073170731707</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.25">
@@ -1376,18 +1376,18 @@
         <v>53</v>
       </c>
       <c r="F41">
-        <v>657</v>
+        <v>632</v>
       </c>
       <c r="G41">
-        <v>304</v>
-      </c>
-      <c r="H41" s="2">
-        <f t="shared" si="0"/>
-        <v>0.77294117647058824</v>
-      </c>
-      <c r="I41" s="2">
-        <f t="shared" si="1"/>
-        <v>0.35764705882352943</v>
+        <v>203</v>
+      </c>
+      <c r="H41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="1"/>
+        <v>0.49512195121951219</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.25">
@@ -1398,18 +1398,18 @@
         <v>53</v>
       </c>
       <c r="F42">
-        <v>657</v>
+        <v>632</v>
       </c>
       <c r="G42">
-        <v>383</v>
-      </c>
-      <c r="H42" s="2">
-        <f t="shared" si="0"/>
-        <v>0.77294117647058824</v>
-      </c>
-      <c r="I42" s="2">
-        <f t="shared" si="1"/>
-        <v>0.45058823529411762</v>
+        <v>281</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.79</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="1"/>
+        <v>0.68536585365853664</v>
       </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.25">
@@ -1420,18 +1420,18 @@
         <v>53</v>
       </c>
       <c r="F43">
-        <v>694</v>
+        <v>669</v>
       </c>
       <c r="G43">
-        <v>346</v>
-      </c>
-      <c r="H43" s="2">
-        <f t="shared" si="0"/>
-        <v>0.81647058823529417</v>
-      </c>
-      <c r="I43" s="2">
-        <f t="shared" si="1"/>
-        <v>0.40705882352941175</v>
+        <v>244</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83625000000000005</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="1"/>
+        <v>0.59512195121951217</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.25">
@@ -1442,18 +1442,18 @@
         <v>53</v>
       </c>
       <c r="F44">
-        <v>691</v>
+        <v>666</v>
       </c>
       <c r="G44">
-        <v>279</v>
-      </c>
-      <c r="H44" s="2">
-        <f t="shared" si="0"/>
-        <v>0.81294117647058828</v>
-      </c>
-      <c r="I44" s="2">
-        <f t="shared" si="1"/>
-        <v>0.32823529411764707</v>
+        <v>177</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="I44" s="1">
+        <f t="shared" si="1"/>
+        <v>0.43170731707317073</v>
       </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.25">
@@ -1464,18 +1464,18 @@
         <v>53</v>
       </c>
       <c r="F45">
-        <v>751</v>
+        <v>726</v>
       </c>
       <c r="G45">
-        <v>343</v>
-      </c>
-      <c r="H45" s="2">
-        <f t="shared" si="0"/>
-        <v>0.8835294117647059</v>
-      </c>
-      <c r="I45" s="2">
-        <f t="shared" si="1"/>
-        <v>0.40352941176470586</v>
+        <v>241</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.90749999999999997</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" si="1"/>
+        <v>0.58780487804878045</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.25">
@@ -1486,18 +1486,18 @@
         <v>53</v>
       </c>
       <c r="F46">
-        <v>785</v>
+        <v>760</v>
       </c>
       <c r="G46">
-        <v>463</v>
-      </c>
-      <c r="H46" s="2">
-        <f t="shared" si="0"/>
-        <v>0.92352941176470593</v>
-      </c>
-      <c r="I46" s="2">
-        <f t="shared" si="1"/>
-        <v>0.54470588235294115</v>
+        <v>361</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88048780487804879</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.25">
@@ -1508,18 +1508,18 @@
         <v>53</v>
       </c>
       <c r="F47">
-        <v>738</v>
+        <v>713</v>
       </c>
       <c r="G47">
-        <v>270</v>
-      </c>
-      <c r="H47" s="2">
-        <f t="shared" si="0"/>
-        <v>0.86823529411764711</v>
-      </c>
-      <c r="I47" s="2">
-        <f t="shared" si="1"/>
-        <v>0.31764705882352939</v>
+        <v>168</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89124999999999999</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40975609756097559</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.25">
@@ -1530,18 +1530,18 @@
         <v>53</v>
       </c>
       <c r="F48">
-        <v>686</v>
+        <v>661</v>
       </c>
       <c r="G48">
-        <v>229</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="0"/>
-        <v>0.80705882352941172</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" si="1"/>
-        <v>0.26941176470588235</v>
+        <v>127</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="0"/>
+        <v>0.82625000000000004</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30975609756097561</v>
       </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.25">
@@ -1552,18 +1552,18 @@
         <v>53</v>
       </c>
       <c r="F49">
-        <v>780</v>
+        <v>755</v>
       </c>
       <c r="G49">
-        <v>253</v>
-      </c>
-      <c r="H49" s="2">
-        <f t="shared" si="0"/>
-        <v>0.91764705882352937</v>
-      </c>
-      <c r="I49" s="2">
-        <f t="shared" si="1"/>
-        <v>0.29764705882352943</v>
+        <v>151</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="0"/>
+        <v>0.94374999999999998</v>
+      </c>
+      <c r="I49" s="1">
+        <f t="shared" si="1"/>
+        <v>0.36829268292682926</v>
       </c>
     </row>
     <row r="50" spans="4:9" x14ac:dyDescent="0.25">
@@ -1574,18 +1574,18 @@
         <v>53</v>
       </c>
       <c r="F50">
-        <v>775</v>
+        <v>750</v>
       </c>
       <c r="G50">
-        <v>209</v>
-      </c>
-      <c r="H50" s="2">
-        <f t="shared" si="0"/>
-        <v>0.91176470588235292</v>
-      </c>
-      <c r="I50" s="2">
-        <f t="shared" si="1"/>
-        <v>0.24588235294117647</v>
+        <v>107</v>
+      </c>
+      <c r="H50" s="1">
+        <f t="shared" si="0"/>
+        <v>0.9375</v>
+      </c>
+      <c r="I50" s="1">
+        <f t="shared" si="1"/>
+        <v>0.26097560975609757</v>
       </c>
     </row>
     <row r="51" spans="4:9" x14ac:dyDescent="0.25">
@@ -1596,18 +1596,18 @@
         <v>53</v>
       </c>
       <c r="F51">
-        <v>734</v>
+        <v>709</v>
       </c>
       <c r="G51">
-        <v>186</v>
-      </c>
-      <c r="H51" s="2">
-        <f t="shared" si="0"/>
-        <v>0.86352941176470588</v>
-      </c>
-      <c r="I51" s="2">
-        <f t="shared" si="1"/>
-        <v>0.21882352941176469</v>
+        <v>84</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="0"/>
+        <v>0.88624999999999998</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="1"/>
+        <v>0.20487804878048779</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.25">
@@ -1618,18 +1618,18 @@
         <v>53</v>
       </c>
       <c r="F52">
-        <v>683</v>
+        <v>657</v>
       </c>
       <c r="G52">
-        <v>188</v>
-      </c>
-      <c r="H52" s="2">
-        <f t="shared" si="0"/>
-        <v>0.80352941176470594</v>
-      </c>
-      <c r="I52" s="2">
-        <f t="shared" si="1"/>
-        <v>0.22117647058823531</v>
+        <v>86</v>
+      </c>
+      <c r="H52" s="1">
+        <f t="shared" si="0"/>
+        <v>0.82125000000000004</v>
+      </c>
+      <c r="I52" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2097560975609756</v>
       </c>
     </row>
   </sheetData>
@@ -1637,6 +1637,6 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>